<commit_message>
Boks. area 20-23 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -106,18 +106,77 @@
   </si>
   <si>
     <t>2022-1</t>
+  </si>
+  <si>
+    <t>2021-3</t>
+  </si>
+  <si>
+    <t>2021-2</t>
+  </si>
+  <si>
+    <t>2021-1</t>
+  </si>
+  <si>
+    <t>2020-3</t>
+  </si>
+  <si>
+    <t>2020-2</t>
+  </si>
+  <si>
+    <t>2020-1</t>
+  </si>
+  <si>
+    <t>2019-3</t>
+  </si>
+  <si>
+    <t>2019-2</t>
+  </si>
+  <si>
+    <t>2019-1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2018-3</t>
+  </si>
+  <si>
+    <t>2018-2</t>
+  </si>
+  <si>
+    <t>2018-1</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>2017-3</t>
+  </si>
+  <si>
+    <t>2017-2</t>
+  </si>
+  <si>
+    <t>2017-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -130,12 +189,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -150,12 +215,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -440,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +604,10 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1">
         <v>2023</v>
       </c>
       <c r="C2" s="2">
@@ -809,10 +880,10 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
         <v>2022</v>
       </c>
       <c r="C6" s="2">
@@ -856,7 +927,7 @@
         <f xml:space="preserve"> 35242373 / 1000</f>
         <v>35242.373</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="3">
         <f xml:space="preserve"> 3936 / 1000</f>
         <v>3.9359999999999999</v>
       </c>
@@ -926,7 +997,7 @@
         <f xml:space="preserve"> 27330488 / 1000</f>
         <v>27330.488000000001</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="3">
         <f xml:space="preserve"> 3936 / 1000</f>
         <v>3.9359999999999999</v>
       </c>
@@ -996,7 +1067,7 @@
         <f xml:space="preserve"> 19111009 / 1000</f>
         <v>19111.008999999998</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="3">
         <f xml:space="preserve"> 3936 / 1000</f>
         <v>3.9359999999999999</v>
       </c>
@@ -1025,466 +1096,1314 @@
       <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="C9" s="2">
+        <v>47.235999999999997</v>
+      </c>
+      <c r="D9" s="2">
+        <v>9.81</v>
+      </c>
+      <c r="E9" s="2">
+        <v>297.5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>53602</v>
+      </c>
+      <c r="G9" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="2">
+        <f xml:space="preserve"> 118255 / 1000</f>
+        <v>118.255</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="2">
+        <f xml:space="preserve"> 9536714 / 1000</f>
+        <v>9536.7139999999999</v>
+      </c>
+      <c r="P9" s="3">
+        <f xml:space="preserve"> 3646 / 1000</f>
+        <v>3.6459999999999999</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S9" s="2">
+        <f xml:space="preserve"> 1192628 / 1000</f>
+        <v>1192.6279999999999</v>
+      </c>
+      <c r="T9" s="2">
+        <f xml:space="preserve"> 64504 / 1000</f>
+        <v>64.504000000000005</v>
+      </c>
+      <c r="U9" s="2">
+        <v>-77</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C10" s="2">
+        <v>48.048000000000002</v>
+      </c>
+      <c r="D10" s="2">
+        <v>10.679</v>
+      </c>
+      <c r="E10" s="2">
+        <v>321.92160000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>50422</v>
+      </c>
+      <c r="G10" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1156.5740000000001</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="2">
+        <v>35244.355000000003</v>
+      </c>
+      <c r="P10" s="2">
+        <f xml:space="preserve"> 5651769 / 1000</f>
+        <v>5651.7690000000002</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S10" s="2">
+        <v>4484.5169999999998</v>
+      </c>
+      <c r="T10" s="2">
+        <v>886.95799999999997</v>
+      </c>
+      <c r="U10" s="2">
+        <v>-39</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
+      <c r="A11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2">
+        <v>48.048000000000002</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10.847</v>
+      </c>
+      <c r="E11" s="2">
+        <v>379.57920000000001</v>
+      </c>
+      <c r="F11" s="2">
+        <v>48483</v>
+      </c>
+      <c r="G11" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="2">
+        <v>979.66600000000005</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="2">
+        <v>29992.044999999998</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2743.337</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S11" s="2">
+        <v>3282.9209999999998</v>
+      </c>
+      <c r="T11" s="2">
+        <v>697.19600000000003</v>
+      </c>
+      <c r="U11" s="2">
+        <v>-2</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2">
+        <v>48.048000000000002</v>
+      </c>
+      <c r="D12" s="2">
+        <v>10.775</v>
+      </c>
+      <c r="E12" s="2">
+        <v>374.77440000000001</v>
+      </c>
+      <c r="F12" s="2">
+        <v>47643</v>
+      </c>
+      <c r="G12" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="2">
+        <v>531.21900000000005</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="2">
+        <v>15612.849</v>
+      </c>
+      <c r="P12" s="2">
+        <v>3150.3989999999999</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S12" s="2">
+        <v>2076.33</v>
+      </c>
+      <c r="T12" s="2">
+        <v>436.51900000000001</v>
+      </c>
+      <c r="U12" s="2">
+        <v>-39</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2">
+        <v>48.048000000000002</v>
+      </c>
+      <c r="D13" s="2">
+        <v>11.242000000000001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>586.18559999999991</v>
+      </c>
+      <c r="F13" s="2">
+        <v>45771</v>
+      </c>
+      <c r="G13" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="2">
+        <v>159.58600000000001</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="2">
+        <v>7291.223</v>
+      </c>
+      <c r="P13" s="2">
+        <v>766.77800000000002</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S13" s="2">
+        <v>965.95899999999995</v>
+      </c>
+      <c r="T13" s="2">
+        <v>187.34200000000001</v>
+      </c>
+      <c r="U13" s="2">
+        <v>-30</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C14" s="2">
+        <v>48.625</v>
+      </c>
+      <c r="D14" s="2">
+        <v>11.957000000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1147.55</v>
+      </c>
+      <c r="F14" s="2">
+        <v>46657</v>
+      </c>
+      <c r="G14" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1532.6489999999999</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="2">
+        <v>28569.743999999999</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1633.874</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" s="2">
+        <v>4092.1239999999998</v>
+      </c>
+      <c r="T14" s="2">
+        <v>799.875</v>
+      </c>
+      <c r="U14" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2">
+        <v>48.625</v>
+      </c>
+      <c r="D15" s="2">
+        <v>12.111000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1312.875</v>
+      </c>
+      <c r="F15" s="2">
+        <v>45571</v>
+      </c>
+      <c r="G15" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="2">
+        <v>781.51300000000003</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="2">
+        <v>20784.951000000001</v>
+      </c>
+      <c r="P15" s="2">
+        <v>990.60799999999995</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S15" s="2">
+        <v>3084.788</v>
+      </c>
+      <c r="T15" s="2">
+        <v>491.70299999999997</v>
+      </c>
+      <c r="U15" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2">
+        <v>48.625</v>
+      </c>
+      <c r="D16" s="2">
+        <v>12.166</v>
+      </c>
+      <c r="E16" s="2">
+        <v>972.5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>44961</v>
+      </c>
+      <c r="G16" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="2">
+        <v>387.61700000000002</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="2">
+        <v>13421.878000000001</v>
+      </c>
+      <c r="P16" s="2">
+        <v>739.61300000000006</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" s="2">
+        <v>2027.5170000000001</v>
+      </c>
+      <c r="T16" s="2">
+        <v>304.42399999999998</v>
+      </c>
+      <c r="U16" s="2">
+        <v>-5</v>
+      </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
+      <c r="A17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2">
+        <v>48.625</v>
+      </c>
+      <c r="D17" s="2">
+        <v>12.096</v>
+      </c>
+      <c r="E17" s="2">
+        <v>325.78750000000002</v>
+      </c>
+      <c r="F17" s="2">
+        <v>46056</v>
+      </c>
+      <c r="G17" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="2">
+        <v>131.001</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="2">
+        <v>6362.3320000000003</v>
+      </c>
+      <c r="P17" s="2">
+        <v>459.274</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S17" s="2">
+        <v>908.74699999999996</v>
+      </c>
+      <c r="T17" s="2">
+        <v>147.86000000000001</v>
+      </c>
+      <c r="U17" s="2">
+        <v>-39</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C18" s="2">
+        <v>49.256</v>
+      </c>
+      <c r="D18" s="2">
+        <v>11.16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>320.16399999999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>47362</v>
+      </c>
+      <c r="G18" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1979.982</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="2">
+        <v>27686.793000000001</v>
+      </c>
+      <c r="P18" s="2">
+        <v>4598.3109999999997</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S18" s="2">
+        <v>3414.6</v>
+      </c>
+      <c r="T18" s="2">
+        <v>358.774</v>
+      </c>
+      <c r="U18" s="2">
+        <v>-99</v>
+      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2">
+        <v>49.256</v>
+      </c>
+      <c r="D19" s="2">
+        <v>10.984999999999999</v>
+      </c>
+      <c r="E19" s="2">
+        <v>315.23840000000001</v>
+      </c>
+      <c r="F19" s="2">
+        <v>46140</v>
+      </c>
+      <c r="G19" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1377.0640000000001</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="2">
+        <v>20678.313999999998</v>
+      </c>
+      <c r="P19" s="2">
+        <v>3786.1819999999998</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S19" s="2">
+        <v>2568.114</v>
+      </c>
+      <c r="T19" s="2">
+        <v>130.35</v>
+      </c>
+      <c r="U19" s="2">
+        <v>-113</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
+        <v>49.256</v>
+      </c>
+      <c r="D20" s="2">
+        <v>10.755000000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>320.10000000000002</v>
+      </c>
+      <c r="F20" s="2">
+        <v>45117</v>
+      </c>
+      <c r="G20" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="2">
+        <f xml:space="preserve"> 998529 / 1000</f>
+        <v>998.529</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="2">
+        <f xml:space="preserve"> 18022751 / 1000</f>
+        <v>18022.751</v>
+      </c>
+      <c r="P20" s="2">
+        <v>2961.0749999999998</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" s="2">
+        <v>1681.731</v>
+      </c>
+      <c r="T20" s="2">
+        <v>62.496000000000002</v>
+      </c>
+      <c r="U20" s="2">
+        <v>-45</v>
+      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="2">
+        <v>49.256</v>
+      </c>
+      <c r="D21" s="2">
+        <v>10.143000000000001</v>
+      </c>
+      <c r="E21" s="2">
+        <v>359.5</v>
+      </c>
+      <c r="F21" s="2">
+        <v>43013</v>
+      </c>
+      <c r="G21" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="2">
+        <v>605.37099999999998</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="2">
+        <v>6387.5039999999999</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1995.894</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="2">
+        <v>801.76199999999994</v>
+      </c>
+      <c r="T21" s="2">
+        <v>47.94</v>
+      </c>
+      <c r="U21" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C22" s="2">
+        <v>50.018999999999998</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9.4879999999999995</v>
+      </c>
+      <c r="E22" s="2">
+        <v>295.1121</v>
+      </c>
+      <c r="F22" s="2">
+        <v>42099</v>
+      </c>
+      <c r="G22" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1362.4960000000001</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="2">
+        <v>25606.316999999999</v>
+      </c>
+      <c r="P22" s="2">
+        <v>2782.0369999999998</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1784.922</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U22" s="2">
+        <v>-186</v>
+      </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
+      <c r="A23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="2">
+        <v>50.018999999999998</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9.4429999999999996</v>
+      </c>
+      <c r="E23" s="2">
+        <v>320.1216</v>
+      </c>
+      <c r="F23" s="2">
+        <v>41710</v>
+      </c>
+      <c r="G23" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="2">
+        <v>933.69399999999996</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="2">
+        <v>18625.789000000001</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1234.4760000000001</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1324.856</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U23" s="2">
+        <v>-8</v>
+      </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2">
+        <v>50.018999999999998</v>
+      </c>
+      <c r="D24" s="2">
+        <v>9.48</v>
+      </c>
+      <c r="E24" s="2">
+        <v>435.16529999999989</v>
+      </c>
+      <c r="F24" s="2">
+        <v>40794</v>
+      </c>
+      <c r="G24" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="2">
+        <v>230.447</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="2">
+        <v>12083.096</v>
+      </c>
+      <c r="P24" s="2">
+        <v>410.03899999999999</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S24" s="2">
+        <v>881.178</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U24" s="2">
+        <v>-29</v>
+      </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
+      <c r="A25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2">
+        <v>50.018999999999998</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9.0440000000000005</v>
+      </c>
+      <c r="E25" s="2">
+        <v>375.14249999999998</v>
+      </c>
+      <c r="F25" s="2">
+        <v>39828</v>
+      </c>
+      <c r="G25" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="2">
+        <v>70.58</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" s="2">
+        <v>5630.76</v>
+      </c>
+      <c r="P25" s="2">
+        <v>24.256</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S25" s="2">
+        <v>430.52600000000001</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U25" s="2">
+        <v>-52</v>
+      </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C26" s="2">
+        <v>50.411999999999999</v>
+      </c>
+      <c r="D26" s="2">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="E26" s="2">
+        <v>362.96640000000002</v>
+      </c>
+      <c r="F26" s="2">
+        <v>37264</v>
+      </c>
+      <c r="G26" s="2">
+        <v>31.3</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1631.1479999999999</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26" s="2">
+        <v>22342.066999999999</v>
+      </c>
+      <c r="P26" s="2">
+        <v>193.648</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="2">
+        <v>1761.789</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U26" s="2">
+        <v>154</v>
+      </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
+      <c r="A27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="2">
+        <v>50.411999999999999</v>
+      </c>
+      <c r="D27" s="2">
+        <v>9.4870000000000001</v>
+      </c>
+      <c r="E27" s="2">
+        <v>368.00760000000002</v>
+      </c>
+      <c r="F27" s="2">
+        <v>36086</v>
+      </c>
+      <c r="G27" s="2">
+        <v>31.3</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1170.4649999999999</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="2">
+        <v>16585.696</v>
+      </c>
+      <c r="P27" s="2">
+        <v>163.39699999999999</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" s="2">
+        <v>1308.778</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U27" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="2">
+        <v>50.411999999999999</v>
+      </c>
+      <c r="D28" s="2">
+        <v>9.5570000000000004</v>
+      </c>
+      <c r="E28" s="2">
+        <v>357.92520000000002</v>
+      </c>
+      <c r="F28" s="2">
+        <v>34804</v>
+      </c>
+      <c r="G28" s="2">
+        <v>31.3</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="2">
+        <v>848.68600000000004</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" s="2">
+        <v>10666.576999999999</v>
+      </c>
+      <c r="P28" s="2">
+        <v>130.45599999999999</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" s="2">
+        <v>861.28899999999999</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U28" s="2">
+        <v>52</v>
+      </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>

</xml_diff>

<commit_message>
Boksitogorsk area 16-19 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -157,18 +157,35 @@
   </si>
   <si>
     <t>2017-1</t>
+  </si>
+  <si>
+    <t>2016-3</t>
+  </si>
+  <si>
+    <t>2016-2</t>
+  </si>
+  <si>
+    <t>2016-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -215,15 +232,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -511,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,117 +2424,319 @@
       <c r="B29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
+      <c r="C29" s="2">
+        <v>50.411999999999999</v>
+      </c>
+      <c r="D29" s="2">
+        <v>9.5730000000000004</v>
+      </c>
+      <c r="E29" s="2">
+        <v>443.62560000000002</v>
+      </c>
+      <c r="F29" s="2">
+        <v>32319</v>
+      </c>
+      <c r="G29" s="2">
+        <v>31.3</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="2">
+        <v>356.84899999999999</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O29" s="2">
+        <v>5313.47</v>
+      </c>
+      <c r="P29" s="2">
+        <v>75.444999999999993</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="2">
+        <v>423.48</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U29" s="2">
+        <v>-47</v>
+      </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
+      <c r="A30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C30" s="2">
+        <v>50.756</v>
+      </c>
+      <c r="D30" s="2">
+        <v>9.8539999999999992</v>
+      </c>
+      <c r="E30" s="2">
+        <v>497.40879999999999</v>
+      </c>
+      <c r="F30" s="2">
+        <v>33918.400000000001</v>
+      </c>
+      <c r="G30" s="2">
+        <v>30.7</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="2">
+        <v>894.31299999999999</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O30" s="2">
+        <v>22261.996999999999</v>
+      </c>
+      <c r="P30" s="2">
+        <v>196.75200000000001</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>5</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S30" s="2">
+        <v>1640.018</v>
+      </c>
+      <c r="T30" s="2">
+        <v>14.432</v>
+      </c>
+      <c r="U30" s="2">
+        <v>169</v>
+      </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
+      <c r="A31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="2">
+        <v>50.756</v>
+      </c>
+      <c r="D31" s="2">
+        <v>9.8770000000000007</v>
+      </c>
+      <c r="E31" s="2">
+        <v>558.31600000000003</v>
+      </c>
+      <c r="F31" s="2">
+        <v>33200.699999999997</v>
+      </c>
+      <c r="G31" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="2">
+        <v>464.42899999999997</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O31" s="2">
+        <v>17010.011999999999</v>
+      </c>
+      <c r="P31" s="2">
+        <v>135.345</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S31" s="2">
+        <v>1232.9459999999999</v>
+      </c>
+      <c r="T31" s="2">
+        <v>10.398</v>
+      </c>
+      <c r="U31" s="2">
+        <v>131</v>
+      </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
+      <c r="A32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="2">
+        <v>50.756</v>
+      </c>
+      <c r="D32" s="2">
+        <v>9.4749999999999996</v>
+      </c>
+      <c r="E32" s="2">
+        <v>497.40879999999999</v>
+      </c>
+      <c r="F32" s="2">
+        <v>32959</v>
+      </c>
+      <c r="G32" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" s="2">
+        <v>246.947</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O32" s="2">
+        <v>11398.271000000001</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S32" s="2">
+        <v>805.52390000000003</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U32" s="2">
+        <v>182</v>
+      </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="A33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="2">
+        <v>50.756</v>
+      </c>
+      <c r="D33" s="2">
+        <v>9.4450000000000003</v>
+      </c>
+      <c r="E33" s="2">
+        <v>588.76959999999997</v>
+      </c>
+      <c r="F33" s="2">
+        <v>32009.5</v>
+      </c>
+      <c r="G33" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" s="2">
+        <v>111.946</v>
+      </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
+      <c r="O33" s="2">
+        <v>4960.6260000000002</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S33" s="2">
+        <v>378.81330000000003</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U33" s="2">
+        <v>65</v>
+      </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>

</xml_diff>

<commit_message>
Boks. city area 13-15 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="56">
   <si>
     <t>name</t>
   </si>
@@ -166,18 +166,55 @@
   </si>
   <si>
     <t>2016-1</t>
+  </si>
+  <si>
+    <t>2015-2</t>
+  </si>
+  <si>
+    <t>2015-1</t>
+  </si>
+  <si>
+    <t>2014-3</t>
+  </si>
+  <si>
+    <t>2014-2</t>
+  </si>
+  <si>
+    <t>2014-1</t>
+  </si>
+  <si>
+    <t>2013-3</t>
+  </si>
+  <si>
+    <t>2013-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -232,15 +269,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -529,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2714,8 +2757,12 @@
       <c r="L33" s="2">
         <v>111.946</v>
       </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="M33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="O33" s="2">
         <v>4960.6260000000002</v>
       </c>
@@ -2739,73 +2786,660 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C34" s="2">
+        <v>51.298000000000002</v>
+      </c>
+      <c r="D34" s="2">
+        <v>9.8369999999999997</v>
+      </c>
+      <c r="E34" s="2">
+        <v>559.14819999999997</v>
+      </c>
+      <c r="F34" s="2">
+        <v>31340.5</v>
+      </c>
+      <c r="G34" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="2">
+        <v>1381.8050000000001</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O34" s="2">
+        <v>19849.96</v>
+      </c>
+      <c r="P34" s="2">
+        <v>159.67099999999999</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S34" s="2">
+        <v>1348.8230000000001</v>
+      </c>
+      <c r="T34" s="2">
+        <v>17.542000000000002</v>
+      </c>
+      <c r="U34" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
+      <c r="A35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="2">
+        <v>51.298000000000002</v>
+      </c>
+      <c r="D35" s="2">
+        <v>9.8420000000000005</v>
+      </c>
+      <c r="E35" s="2">
+        <v>528.36940000000004</v>
+      </c>
+      <c r="F35" s="2">
+        <v>30168.3</v>
+      </c>
+      <c r="G35" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" s="2">
+        <v>375.24799999999999</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O35" s="2">
+        <v>8921.6020000000008</v>
+      </c>
+      <c r="P35" s="2">
+        <v>97.123000000000005</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S35" s="2">
+        <v>646.63130000000001</v>
+      </c>
+      <c r="T35" s="2">
+        <v>7.9740000000000002</v>
+      </c>
+      <c r="U35" s="2">
+        <v>-47</v>
+      </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
+      <c r="A36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="2">
+        <v>51.298000000000002</v>
+      </c>
+      <c r="D36" s="2">
+        <v>9.484</v>
+      </c>
+      <c r="E36" s="2">
+        <v>651.4846</v>
+      </c>
+      <c r="F36" s="2">
+        <v>29247</v>
+      </c>
+      <c r="G36" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="2">
+        <v>233.422</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O36" s="2">
+        <v>4239.7669999999998</v>
+      </c>
+      <c r="P36" s="2">
+        <v>72.281999999999996</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S36" s="2">
+        <v>310.39400000000001</v>
+      </c>
+      <c r="T36" s="2">
+        <v>3.1280000000000001</v>
+      </c>
+      <c r="U36" s="2">
+        <v>-88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C37" s="2">
+        <v>51.941000000000003</v>
+      </c>
+      <c r="D37" s="2">
+        <v>9.9879999999999995</v>
+      </c>
+      <c r="E37" s="2">
+        <v>597.32150000000001</v>
+      </c>
+      <c r="F37" s="2">
+        <v>28366.2</v>
+      </c>
+      <c r="G37" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="2">
+        <v>814.22699999999998</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O37" s="2">
+        <v>17254.972000000002</v>
+      </c>
+      <c r="P37" s="2">
+        <v>173.51900000000001</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S37" s="2">
+        <v>967.63780000000008</v>
+      </c>
+      <c r="T37" s="2">
+        <v>16.149000000000001</v>
+      </c>
+      <c r="U37" s="2">
+        <v>-257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="2">
+        <v>51.941000000000003</v>
+      </c>
+      <c r="D38" s="2">
+        <v>9.6289999999999996</v>
+      </c>
+      <c r="E38" s="2">
+        <v>571.35100000000011</v>
+      </c>
+      <c r="F38" s="2">
+        <v>27629.3</v>
+      </c>
+      <c r="G38" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="2">
+        <v>539.61500000000001</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O38" s="2">
+        <v>13057.217000000001</v>
+      </c>
+      <c r="P38" s="2">
+        <v>121.94</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S38" s="2">
+        <v>713.79509999999993</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U38" s="2">
+        <v>-296</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="2">
+        <v>51.941000000000003</v>
+      </c>
+      <c r="D39" s="2">
+        <v>9.6869999999999994</v>
+      </c>
+      <c r="E39" s="2">
+        <v>649.26250000000005</v>
+      </c>
+      <c r="F39" s="2">
+        <v>27227.599999999999</v>
+      </c>
+      <c r="G39" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="2">
+        <v>348.56700000000001</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O39" s="2">
+        <v>8391.2710000000006</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S39" s="2">
+        <v>462.08280000000002</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U39" s="2">
+        <v>-133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="2">
+        <v>51.941000000000003</v>
+      </c>
+      <c r="D40" s="2">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="E40" s="2">
+        <v>711.59170000000006</v>
+      </c>
+      <c r="F40" s="2">
+        <v>26575.1</v>
+      </c>
+      <c r="G40" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40" s="2">
+        <v>104.276</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O40" s="2">
+        <v>3715.451</v>
+      </c>
+      <c r="P40" s="2">
+        <v>29.863</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S40" s="2">
+        <v>210.19110000000001</v>
+      </c>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2">
+        <v>-117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2013</v>
+      </c>
+      <c r="C41" s="2">
+        <v>52.34</v>
+      </c>
+      <c r="D41" s="2">
+        <v>10.254</v>
+      </c>
+      <c r="E41" s="2">
+        <v>711.82400000000007</v>
+      </c>
+      <c r="F41" s="2">
+        <v>25409.8</v>
+      </c>
+      <c r="G41" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L41" s="2">
+        <v>691.16099999999994</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O41" s="2">
+        <v>17653.433000000001</v>
+      </c>
+      <c r="P41" s="2">
+        <v>85.984999999999999</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S41" s="2">
+        <v>821.76700000000005</v>
+      </c>
+      <c r="T41" s="2">
+        <v>24.484999999999999</v>
+      </c>
+      <c r="U41" s="2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="2">
+        <v>52.34</v>
+      </c>
+      <c r="D42" s="2">
+        <v>10.311999999999999</v>
+      </c>
+      <c r="E42" s="2">
+        <v>732.75999999999988</v>
+      </c>
+      <c r="F42" s="2">
+        <v>24734.2</v>
+      </c>
+      <c r="G42" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" s="2">
+        <v>470.82900000000001</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O42" s="2">
+        <v>13476.197</v>
+      </c>
+      <c r="P42" s="2">
+        <v>70.808000000000007</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S42" s="2">
+        <v>602.79399999999998</v>
+      </c>
+      <c r="T42" s="2">
+        <v>20.125</v>
+      </c>
+      <c r="U42" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="2">
+        <v>52.347000000000001</v>
+      </c>
+      <c r="D43" s="2">
+        <v>10.744</v>
+      </c>
+      <c r="E43" s="2">
+        <v>790.43970000000002</v>
+      </c>
+      <c r="F43" s="2">
+        <v>24480.9</v>
+      </c>
+      <c r="G43" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" s="2">
+        <v>306.81</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O43" s="2">
+        <v>8461.3485999999994</v>
+      </c>
+      <c r="P43" s="2">
+        <v>13.167</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S43" s="2">
+        <v>381.46929999999998</v>
+      </c>
+      <c r="T43" s="2">
+        <v>13.260999999999999</v>
+      </c>
+      <c r="U43" s="2">
+        <v>-22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2012</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Boks. city area 11-12 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -187,18 +187,41 @@
   </si>
   <si>
     <t>2013-2</t>
+  </si>
+  <si>
+    <t>2012-3</t>
+  </si>
+  <si>
+    <t>2012-2</t>
+  </si>
+  <si>
+    <t>2012-1</t>
+  </si>
+  <si>
+    <t>2011-3</t>
+  </si>
+  <si>
+    <t>2011-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -269,15 +292,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -572,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3440,6 +3466,458 @@
       <c r="B44" s="1">
         <v>2012</v>
       </c>
+      <c r="C44" s="2">
+        <v>52.956000000000003</v>
+      </c>
+      <c r="D44" s="2">
+        <v>10.59</v>
+      </c>
+      <c r="E44" s="2">
+        <v>751.97519999999997</v>
+      </c>
+      <c r="F44" s="2">
+        <v>23164</v>
+      </c>
+      <c r="G44" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L44" s="2">
+        <v>955.6</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O44" s="2">
+        <v>16316.396500000001</v>
+      </c>
+      <c r="P44" s="2">
+        <v>230.62899999999999</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S44" s="2">
+        <v>714.0385</v>
+      </c>
+      <c r="T44" s="2">
+        <v>32.409999999999997</v>
+      </c>
+      <c r="U44" s="2">
+        <v>-76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="2">
+        <v>52.956000000000003</v>
+      </c>
+      <c r="D45" s="2">
+        <v>10.656000000000001</v>
+      </c>
+      <c r="E45" s="2">
+        <v>820.81799999999998</v>
+      </c>
+      <c r="F45" s="2">
+        <v>22678.7</v>
+      </c>
+      <c r="G45" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L45" s="2">
+        <v>555.20000000000005</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O45" s="2">
+        <v>12156.020200000001</v>
+      </c>
+      <c r="P45" s="2">
+        <v>213.245</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S45" s="2">
+        <v>541.29999999999995</v>
+      </c>
+      <c r="T45" s="2">
+        <v>25.183</v>
+      </c>
+      <c r="U45" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="2">
+        <v>52.956000000000003</v>
+      </c>
+      <c r="D46" s="2">
+        <v>10.754</v>
+      </c>
+      <c r="E46" s="2">
+        <v>905.54759999999999</v>
+      </c>
+      <c r="F46" s="2">
+        <v>22481.9</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L46" s="2">
+        <v>392.56200000000001</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O46" s="2">
+        <v>8008.607</v>
+      </c>
+      <c r="P46" s="2">
+        <v>42.528500000000001</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>1.2602</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S46" s="2">
+        <v>358.3</v>
+      </c>
+      <c r="T46" s="2">
+        <v>15.971</v>
+      </c>
+      <c r="U46" s="2">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="2">
+        <v>52.956000000000003</v>
+      </c>
+      <c r="D47" s="2">
+        <v>10.856999999999999</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1080.3024</v>
+      </c>
+      <c r="F47" s="2">
+        <v>21849.8</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L47" s="2">
+        <v>157.38900000000001</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O47" s="2">
+        <v>3812.3490000000002</v>
+      </c>
+      <c r="P47" s="2">
+        <v>2.0089999999999999</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S47" s="2">
+        <v>167.21520000000001</v>
+      </c>
+      <c r="T47" s="2">
+        <v>7.5609999999999999</v>
+      </c>
+      <c r="U47" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2011</v>
+      </c>
+      <c r="C48" s="2">
+        <v>53.338000000000001</v>
+      </c>
+      <c r="D48" s="2">
+        <v>11.303000000000001</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1002.7544</v>
+      </c>
+      <c r="F48" s="2">
+        <v>20279</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L48" s="2">
+        <v>577.28300000000002</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O48" s="2">
+        <v>15980.2601</v>
+      </c>
+      <c r="P48" s="2">
+        <v>309.06599999999997</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S48" s="2">
+        <v>633.4</v>
+      </c>
+      <c r="T48" s="2">
+        <v>29.247</v>
+      </c>
+      <c r="U48" s="2">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="2">
+        <v>53.338000000000001</v>
+      </c>
+      <c r="D49" s="2">
+        <v>11.781000000000001</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1008.0882</v>
+      </c>
+      <c r="F49" s="2">
+        <v>20072.7</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L49" s="2">
+        <v>388.98500000000001</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O49" s="2">
+        <v>12270.528399999999</v>
+      </c>
+      <c r="P49" s="2">
+        <v>164.96899999999999</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S49" s="2">
+        <v>106</v>
+      </c>
+      <c r="T49" s="2">
+        <v>20.931999999999999</v>
+      </c>
+      <c r="U49" s="2">
+        <v>-113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="2">
+        <v>53.338000000000001</v>
+      </c>
+      <c r="D50" s="2">
+        <v>11.946</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1050.7585999999999</v>
+      </c>
+      <c r="F50" s="2">
+        <v>19232.8</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L50" s="2">
+        <v>231.96799999999999</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O50" s="2">
+        <v>7600.5610999999999</v>
+      </c>
+      <c r="P50" s="2">
+        <v>49.552</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>1.68</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S50" s="2">
+        <v>300</v>
+      </c>
+      <c r="T50" s="2">
+        <v>12.555</v>
+      </c>
+      <c r="U50" s="2">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gatchina area 19-17 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>2011-2</t>
+  </si>
+  <si>
+    <t>Гатчинский МР</t>
   </si>
 </sst>
 </file>
@@ -598,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3915,9 +3918,205 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="2"/>
+      <c r="A51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C51" s="2">
+        <v>238.018</v>
+      </c>
+      <c r="D51" s="2">
+        <v>42.329000000000001</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1035</v>
+      </c>
+      <c r="F51" s="2">
+        <v>47095.7</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L51" s="2">
+        <v>8534.4</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N51" s="2">
+        <v>8877</v>
+      </c>
+      <c r="O51" s="2">
+        <v>98966.3</v>
+      </c>
+      <c r="P51" s="2">
+        <v>10252.700000000001</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>88.7</v>
+      </c>
+      <c r="R51" s="2">
+        <v>29</v>
+      </c>
+      <c r="S51" s="2">
+        <f xml:space="preserve"> 22883164.3 / 1000</f>
+        <v>22883.1643</v>
+      </c>
+      <c r="T51" s="2">
+        <f xml:space="preserve"> 353488 / 1000</f>
+        <v>353.488</v>
+      </c>
+      <c r="U51" s="2">
+        <v>-3761</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C52" s="2">
+        <v>243.17</v>
+      </c>
+      <c r="D52" s="2">
+        <v>43.061</v>
+      </c>
+      <c r="E52" s="2">
+        <v>836</v>
+      </c>
+      <c r="F52" s="2">
+        <v>43057.3</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L52" s="2">
+        <v>19293.900000000001</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N52" s="2">
+        <v>8284</v>
+      </c>
+      <c r="O52" s="2">
+        <v>81900</v>
+      </c>
+      <c r="P52" s="2">
+        <v>8500</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>142.5</v>
+      </c>
+      <c r="R52" s="2">
+        <v>646</v>
+      </c>
+      <c r="S52" s="2">
+        <f xml:space="preserve"> 16022223.4 / 1000</f>
+        <v>16022.223400000001</v>
+      </c>
+      <c r="T52" s="2">
+        <f xml:space="preserve"> 171538.4 / 1000</f>
+        <v>171.5384</v>
+      </c>
+      <c r="U52" s="2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C53" s="2">
+        <v>244.25800000000001</v>
+      </c>
+      <c r="D53" s="2">
+        <v>37.133000000000003</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1006</v>
+      </c>
+      <c r="F53" s="2">
+        <v>41288</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L53" s="2">
+        <v>6649.3</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N53" s="2">
+        <v>7663</v>
+      </c>
+      <c r="O53" s="2">
+        <v>63344.5</v>
+      </c>
+      <c r="P53" s="2">
+        <v>2696.5</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>165.1</v>
+      </c>
+      <c r="R53" s="2">
+        <v>1535</v>
+      </c>
+      <c r="S53" s="2">
+        <f xml:space="preserve"> 14877213.8 / 1000</f>
+        <v>14877.213800000001</v>
+      </c>
+      <c r="T53" s="2">
+        <f xml:space="preserve"> 132601 / 1000</f>
+        <v>132.601</v>
+      </c>
+      <c r="U53" s="2">
+        <v>-63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gatchina area 14-16 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -295,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,6 +319,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -601,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O55" sqref="O55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3957,8 +3960,8 @@
       <c r="M51" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N51" s="2">
-        <v>8877</v>
+      <c r="N51" s="3">
+        <v>11911</v>
       </c>
       <c r="O51" s="2">
         <v>98966.3</v>
@@ -3970,7 +3973,7 @@
         <v>88.7</v>
       </c>
       <c r="R51" s="2">
-        <v>29</v>
+        <v>1340</v>
       </c>
       <c r="S51" s="2">
         <f xml:space="preserve"> 22883164.3 / 1000</f>
@@ -4024,8 +4027,8 @@
       <c r="M52" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N52" s="2">
-        <v>8284</v>
+      <c r="N52" s="3">
+        <v>11312</v>
       </c>
       <c r="O52" s="2">
         <v>81900</v>
@@ -4091,8 +4094,8 @@
       <c r="M53" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N53" s="2">
-        <v>7663</v>
+      <c r="N53" s="3">
+        <v>10838</v>
       </c>
       <c r="O53" s="2">
         <v>63344.5</v>
@@ -4116,6 +4119,196 @@
       </c>
       <c r="U53" s="2">
         <v>-63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C54" s="2">
+        <v>245.60599999999999</v>
+      </c>
+      <c r="D54" s="2">
+        <v>36.497999999999998</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1156</v>
+      </c>
+      <c r="F54" s="2">
+        <v>37629.5</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L54" s="2">
+        <v>7320.8</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N54" s="3">
+        <v>10551</v>
+      </c>
+      <c r="O54" s="2">
+        <v>60117.7</v>
+      </c>
+      <c r="P54" s="2">
+        <v>1270</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="R54" s="2">
+        <v>1684</v>
+      </c>
+      <c r="S54" s="2">
+        <f xml:space="preserve"> 13562423.7 / 1000</f>
+        <v>13562.423699999999</v>
+      </c>
+      <c r="T54" s="2">
+        <f xml:space="preserve"> 128209.1 / 1000</f>
+        <v>128.20910000000001</v>
+      </c>
+      <c r="U54" s="2">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C55" s="2">
+        <v>246</v>
+      </c>
+      <c r="D55" s="2">
+        <v>36.811</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1380</v>
+      </c>
+      <c r="F55" s="2">
+        <v>34278.9</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L55" s="2">
+        <v>7689.2</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N55" s="3">
+        <v>10455</v>
+      </c>
+      <c r="O55" s="2">
+        <v>57475.199999999997</v>
+      </c>
+      <c r="P55" s="2">
+        <v>2335.9</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>181.1</v>
+      </c>
+      <c r="R55" s="2">
+        <v>2530</v>
+      </c>
+      <c r="S55" s="2">
+        <v>31739</v>
+      </c>
+      <c r="T55" s="9">
+        <v>722</v>
+      </c>
+      <c r="U55" s="2">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C56" s="2">
+        <v>246.2</v>
+      </c>
+      <c r="D56" s="2">
+        <v>37.902999999999999</v>
+      </c>
+      <c r="E56" s="2">
+        <v>763</v>
+      </c>
+      <c r="F56" s="2">
+        <v>32674.7</v>
+      </c>
+      <c r="G56" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="L56">
+        <f xml:space="preserve"> 4558593 / 1000</f>
+        <v>4558.5929999999998</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56" s="2">
+        <f xml:space="preserve"> 41975492 / 1000</f>
+        <v>41975.491999999998</v>
+      </c>
+      <c r="P56" s="2">
+        <f xml:space="preserve"> 3280900 / 1000</f>
+        <v>3280.9</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>123.8</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S56" s="2">
+        <f xml:space="preserve"> 10145823.2 / 1000</f>
+        <v>10145.823199999999</v>
+      </c>
+      <c r="T56" s="2">
+        <f xml:space="preserve"> 119837 / 1000</f>
+        <v>119.837</v>
+      </c>
+      <c r="U56" s="2">
+        <v>3215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gatchina city 17-19 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Гатчинский МР</t>
+  </si>
+  <si>
+    <t>Гатчина</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,6 +331,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -604,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,10 +4284,22 @@
       <c r="F56" s="2">
         <v>32674.7</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="10">
         <v>25.9</v>
       </c>
-      <c r="L56">
+      <c r="H56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L56" s="2">
         <f xml:space="preserve"> 4558593 / 1000</f>
         <v>4558.5929999999998</v>
       </c>
@@ -4309,6 +4333,207 @@
       </c>
       <c r="U56" s="2">
         <v>3215</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C57" s="2">
+        <v>91.677999999999997</v>
+      </c>
+      <c r="D57" s="2">
+        <v>27.295000000000002</v>
+      </c>
+      <c r="E57" s="2">
+        <v>189</v>
+      </c>
+      <c r="F57" s="2">
+        <v>45526</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L57" s="2">
+        <v>3022.6</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" s="3">
+        <v>5566</v>
+      </c>
+      <c r="O57" s="2">
+        <v>22280.27</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S57" s="2">
+        <f>21358889.6/1000</f>
+        <v>21358.889600000002</v>
+      </c>
+      <c r="T57" s="2">
+        <f>333725.2/1000</f>
+        <v>333.72520000000003</v>
+      </c>
+      <c r="U57" s="2">
+        <v>-1280</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C58" s="2">
+        <v>93.721999999999994</v>
+      </c>
+      <c r="D58" s="2">
+        <v>27.602</v>
+      </c>
+      <c r="E58" s="2">
+        <v>144</v>
+      </c>
+      <c r="F58" s="2">
+        <v>41230.699999999997</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L58" s="2">
+        <v>12843.2</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N58" s="3">
+        <v>5245</v>
+      </c>
+      <c r="O58" s="2">
+        <v>33385.4</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S58" s="2">
+        <f>15613892/1000</f>
+        <v>15613.892</v>
+      </c>
+      <c r="T58" s="2">
+        <f>170054/1000</f>
+        <v>170.054</v>
+      </c>
+      <c r="U58" s="2">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C59" s="2">
+        <v>94.45</v>
+      </c>
+      <c r="D59" s="2">
+        <v>22.256</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1006</v>
+      </c>
+      <c r="F59" s="2">
+        <v>41319.300000000003</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L59" s="2">
+        <v>2983.3</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N59" s="3">
+        <v>5071</v>
+      </c>
+      <c r="O59" s="2">
+        <v>26147.7</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S59" s="2">
+        <f xml:space="preserve"> 9892900 / 1000</f>
+        <v>9892.9</v>
+      </c>
+      <c r="T59" s="2">
+        <f xml:space="preserve"> 130235 / 1000</f>
+        <v>130.23500000000001</v>
+      </c>
+      <c r="U59" s="2">
+        <v>-114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gatchina city 2016 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -616,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U59"/>
+  <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4536,6 +4536,73 @@
         <v>-114</v>
       </c>
     </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C60" s="2">
+        <v>95.177999999999997</v>
+      </c>
+      <c r="D60" s="2">
+        <v>21.986999999999998</v>
+      </c>
+      <c r="E60" s="2">
+        <v>230</v>
+      </c>
+      <c r="F60" s="2">
+        <v>38178.1</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L60" s="2">
+        <v>4169.8</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N60" s="3">
+        <v>4979</v>
+      </c>
+      <c r="O60" s="2">
+        <v>25080.5</v>
+      </c>
+      <c r="P60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S60" s="2">
+        <f>9719218.2/1000</f>
+        <v>9719.2181999999993</v>
+      </c>
+      <c r="T60" s="2">
+        <f xml:space="preserve"> 123943/1000</f>
+        <v>123.943</v>
+      </c>
+      <c r="U60" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Vyborg area 21-23 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Гатчина</t>
+  </si>
+  <si>
+    <t>Выборгский МР</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +294,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -304,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -334,6 +343,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -616,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U60"/>
+  <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R51" sqref="R51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,8 +652,7 @@
     <col min="16" max="16" width="12.140625" customWidth="1"/>
     <col min="17" max="17" width="16.28515625" customWidth="1"/>
     <col min="18" max="18" width="16.140625" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="20" width="22.140625" customWidth="1"/>
+    <col min="19" max="20" width="17.42578125" customWidth="1"/>
     <col min="21" max="21" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3951,8 +3962,8 @@
       <c r="F51" s="2">
         <v>47095.7</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>22</v>
+      <c r="G51" s="10">
+        <v>25.9</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>22</v>
@@ -4018,8 +4029,8 @@
       <c r="F52" s="2">
         <v>43057.3</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>22</v>
+      <c r="G52" s="10">
+        <v>25.9</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>22</v>
@@ -4085,8 +4096,8 @@
       <c r="F53" s="2">
         <v>41288</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>22</v>
+      <c r="G53" s="10">
+        <v>25.9</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>22</v>
@@ -4152,8 +4163,8 @@
       <c r="F54" s="2">
         <v>37629.5</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>22</v>
+      <c r="G54" s="10">
+        <v>25.9</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>22</v>
@@ -4219,8 +4230,8 @@
       <c r="F55" s="2">
         <v>34278.9</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>22</v>
+      <c r="G55" s="10">
+        <v>25.9</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>22</v>
@@ -4601,6 +4612,209 @@
       </c>
       <c r="U60" s="2">
         <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C61" s="2">
+        <v>194.703</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="2">
+        <v>756</v>
+      </c>
+      <c r="F61" s="2">
+        <v>77711</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L61" s="11">
+        <f>32741549/1000</f>
+        <v>32741.548999999999</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N61" s="3">
+        <v>6928</v>
+      </c>
+      <c r="O61" s="11">
+        <f xml:space="preserve"> 188.5 * 1000</f>
+        <v>188500</v>
+      </c>
+      <c r="P61" s="2">
+        <f>2.8*1000</f>
+        <v>2800</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>301.2</v>
+      </c>
+      <c r="R61" s="2">
+        <v>2056</v>
+      </c>
+      <c r="S61" s="2">
+        <v>34208.9</v>
+      </c>
+      <c r="T61" s="2">
+        <v>859</v>
+      </c>
+      <c r="U61" s="2">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C62" s="2">
+        <v>192.55699999999999</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="2">
+        <v>983</v>
+      </c>
+      <c r="F62" s="2">
+        <v>69206</v>
+      </c>
+      <c r="G62" s="10">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L62" s="11">
+        <f>22754436/1000</f>
+        <v>22754.436000000002</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N62" s="3">
+        <v>6566</v>
+      </c>
+      <c r="O62" s="11">
+        <f xml:space="preserve"> 172 * 1000</f>
+        <v>172000</v>
+      </c>
+      <c r="P62" s="9">
+        <v>3002.7</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>282.5</v>
+      </c>
+      <c r="R62" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S62" s="2">
+        <f xml:space="preserve"> 33764801.6 /1000</f>
+        <v>33764.801599999999</v>
+      </c>
+      <c r="T62" s="2">
+        <f xml:space="preserve"> 775672.3 / 1000</f>
+        <v>775.67230000000006</v>
+      </c>
+      <c r="U62" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C63" s="2">
+        <v>193.827</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1443</v>
+      </c>
+      <c r="F63" s="2">
+        <v>61131</v>
+      </c>
+      <c r="G63" s="10">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L63" s="11">
+        <f>19495388/1000</f>
+        <v>19495.387999999999</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N63" s="3">
+        <v>6511</v>
+      </c>
+      <c r="O63" s="11">
+        <f xml:space="preserve"> 152.7 * 1000</f>
+        <v>152700</v>
+      </c>
+      <c r="P63" s="2">
+        <v>5924.4</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>321.89999999999998</v>
+      </c>
+      <c r="R63" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S63" s="2">
+        <f xml:space="preserve"> 30160128.5 /1000</f>
+        <v>30160.128499999999</v>
+      </c>
+      <c r="T63" s="2">
+        <f xml:space="preserve"> 710657.1 /1000</f>
+        <v>710.65710000000001</v>
+      </c>
+      <c r="U63" s="2">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vyborg area 17-20 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -275,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,12 +294,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -313,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,9 +337,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4624,8 +4615,8 @@
       <c r="C61" s="2">
         <v>194.703</v>
       </c>
-      <c r="D61" s="11" t="s">
-        <v>22</v>
+      <c r="D61" s="9">
+        <v>41.1</v>
       </c>
       <c r="E61" s="2">
         <v>756</v>
@@ -4648,7 +4639,7 @@
       <c r="K61" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L61" s="11">
+      <c r="L61" s="9">
         <f>32741549/1000</f>
         <v>32741.548999999999</v>
       </c>
@@ -4658,7 +4649,7 @@
       <c r="N61" s="3">
         <v>6928</v>
       </c>
-      <c r="O61" s="11">
+      <c r="O61" s="9">
         <f xml:space="preserve"> 188.5 * 1000</f>
         <v>188500</v>
       </c>
@@ -4692,8 +4683,8 @@
       <c r="C62" s="2">
         <v>192.55699999999999</v>
       </c>
-      <c r="D62" s="11" t="s">
-        <v>22</v>
+      <c r="D62" s="9">
+        <v>42.4</v>
       </c>
       <c r="E62" s="2">
         <v>983</v>
@@ -4701,7 +4692,7 @@
       <c r="F62" s="2">
         <v>69206</v>
       </c>
-      <c r="G62" s="10">
+      <c r="G62" s="9">
         <v>32.299999999999997</v>
       </c>
       <c r="H62" s="2" t="s">
@@ -4716,7 +4707,7 @@
       <c r="K62" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L62" s="11">
+      <c r="L62" s="9">
         <f>22754436/1000</f>
         <v>22754.436000000002</v>
       </c>
@@ -4726,7 +4717,7 @@
       <c r="N62" s="3">
         <v>6566</v>
       </c>
-      <c r="O62" s="11">
+      <c r="O62" s="9">
         <f xml:space="preserve"> 172 * 1000</f>
         <v>172000</v>
       </c>
@@ -4761,13 +4752,16 @@
       <c r="C63" s="2">
         <v>193.827</v>
       </c>
+      <c r="D63" s="9">
+        <v>41.5</v>
+      </c>
       <c r="E63" s="2">
         <v>1443</v>
       </c>
       <c r="F63" s="2">
         <v>61131</v>
       </c>
-      <c r="G63" s="10">
+      <c r="G63" s="9">
         <v>32.299999999999997</v>
       </c>
       <c r="H63" s="2" t="s">
@@ -4782,7 +4776,7 @@
       <c r="K63" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L63" s="11">
+      <c r="L63" s="9">
         <f>19495388/1000</f>
         <v>19495.387999999999</v>
       </c>
@@ -4792,7 +4786,7 @@
       <c r="N63" s="3">
         <v>6511</v>
       </c>
-      <c r="O63" s="11">
+      <c r="O63" s="9">
         <f xml:space="preserve"> 152.7 * 1000</f>
         <v>152700</v>
       </c>
@@ -4815,6 +4809,284 @@
       </c>
       <c r="U63" s="2">
         <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C64" s="2">
+        <v>195.833</v>
+      </c>
+      <c r="D64" s="9">
+        <v>41</v>
+      </c>
+      <c r="E64" s="2">
+        <v>4324</v>
+      </c>
+      <c r="F64" s="2">
+        <v>56640</v>
+      </c>
+      <c r="G64" s="9">
+        <v>29.3</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L64" s="9">
+        <v>37458.699999999997</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N64" s="3">
+        <v>6442</v>
+      </c>
+      <c r="O64" s="9">
+        <f xml:space="preserve"> 110.9 * 1000</f>
+        <v>110900</v>
+      </c>
+      <c r="P64" s="2">
+        <f xml:space="preserve"> 1589809 / 1000</f>
+        <v>1589.809</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>192.6</v>
+      </c>
+      <c r="R64" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S64" s="2">
+        <f>27435002/1000</f>
+        <v>27435.002</v>
+      </c>
+      <c r="T64" s="2">
+        <f xml:space="preserve"> 368788.4/1000</f>
+        <v>368.78840000000002</v>
+      </c>
+      <c r="U64" s="2">
+        <v>-907</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C65" s="2">
+        <v>198.22900000000001</v>
+      </c>
+      <c r="D65" s="9">
+        <v>42.8</v>
+      </c>
+      <c r="E65" s="2">
+        <v>813</v>
+      </c>
+      <c r="F65" s="2">
+        <v>55350</v>
+      </c>
+      <c r="G65" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L65" s="9">
+        <f>21049559/1000</f>
+        <v>21049.559000000001</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N65" s="3">
+        <v>6476</v>
+      </c>
+      <c r="O65" s="9">
+        <f>101*1000</f>
+        <v>101000</v>
+      </c>
+      <c r="P65" s="2">
+        <f xml:space="preserve"> 1573240 / 1000</f>
+        <v>1573.24</v>
+      </c>
+      <c r="Q65" s="2">
+        <v>193.08</v>
+      </c>
+      <c r="R65" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S65" s="2">
+        <f>24726130.6/1000</f>
+        <v>24726.1306</v>
+      </c>
+      <c r="T65" s="2">
+        <f>482383/1000</f>
+        <v>482.38299999999998</v>
+      </c>
+      <c r="U65" s="2">
+        <v>-212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C66" s="2">
+        <v>199.61099999999999</v>
+      </c>
+      <c r="D66" s="9">
+        <v>42.3</v>
+      </c>
+      <c r="E66" s="2">
+        <v>648</v>
+      </c>
+      <c r="F66" s="2">
+        <v>51266</v>
+      </c>
+      <c r="G66" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L66" s="2">
+        <f>26707512/1000</f>
+        <v>26707.511999999999</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N66" s="3">
+        <v>6584</v>
+      </c>
+      <c r="O66" s="9">
+        <f>105.7*1000</f>
+        <v>105700</v>
+      </c>
+      <c r="P66">
+        <f>4153307.4/1000</f>
+        <v>4153.3073999999997</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>121.1</v>
+      </c>
+      <c r="R66" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S66" s="2">
+        <f>14607097.9/1000</f>
+        <v>14607.097900000001</v>
+      </c>
+      <c r="T66" s="2">
+        <f>114827.7/1000</f>
+        <v>114.82769999999999</v>
+      </c>
+      <c r="U66" s="2">
+        <v>-440</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C67" s="2">
+        <v>201.232</v>
+      </c>
+      <c r="D67" s="9">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="E67" s="2">
+        <v>786</v>
+      </c>
+      <c r="F67" s="2">
+        <v>45530</v>
+      </c>
+      <c r="G67" s="2">
+        <v>26.9</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L67" s="2">
+        <f>7232770/1000</f>
+        <v>7232.77</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N67" s="3">
+        <v>8968</v>
+      </c>
+      <c r="O67" s="2">
+        <f>65.7 *1000</f>
+        <v>65700</v>
+      </c>
+      <c r="P67" s="2">
+        <v>562.70000000000005</v>
+      </c>
+      <c r="Q67" s="2">
+        <v>102.3</v>
+      </c>
+      <c r="R67" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S67" s="2">
+        <f>14037631.3/1000</f>
+        <v>14037.631300000001</v>
+      </c>
+      <c r="T67" s="2">
+        <f>76884.3/1000</f>
+        <v>76.884299999999996</v>
+      </c>
+      <c r="U67" s="2">
+        <v>-550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slantsy city 14-15 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -107,25 +107,20 @@
   <si>
     <t>Выборг</t>
   </si>
+  <si>
+    <t>Сланцы</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,15 +184,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -213,7 +205,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -498,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +698,7 @@
         <f xml:space="preserve"> 35242373 / 1000</f>
         <v>35242.373</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="6">
         <f xml:space="preserve"> 3936 / 1000</f>
         <v>3.9359999999999999</v>
       </c>
@@ -774,7 +766,7 @@
       <c r="O4" s="2">
         <v>35244.355000000003</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="6">
         <f xml:space="preserve"> 5651769 / 1000</f>
         <v>5651.7690000000002</v>
       </c>
@@ -840,7 +832,7 @@
       <c r="O5" s="2">
         <v>28569.743999999999</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="6">
         <v>1633.874</v>
       </c>
       <c r="Q5" s="2" t="s">
@@ -1463,43 +1455,43 @@
       <c r="F15" s="2">
         <v>47095.7</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>25.9</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="7">
+      <c r="H15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="6">
         <v>8534.4</v>
       </c>
-      <c r="M15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="7">
+      <c r="M15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="6">
         <v>11911</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="6">
         <v>98966.3</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="6">
         <v>10252.700000000001</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="6">
         <v>88.7</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="6">
         <v>1340</v>
       </c>
-      <c r="S15" s="7">
+      <c r="S15" s="6">
         <f xml:space="preserve"> 22883164.3 / 1000</f>
         <v>22883.1643</v>
       </c>
@@ -1530,43 +1522,43 @@
       <c r="F16" s="2">
         <v>43057.3</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>25.9</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="7">
+      <c r="H16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="6">
         <v>19293.900000000001</v>
       </c>
-      <c r="M16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="7">
+      <c r="M16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="6">
         <v>11312</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="6">
         <v>81900</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="6">
         <v>8500</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="6">
         <v>142.5</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16" s="6">
         <v>646</v>
       </c>
-      <c r="S16" s="7">
+      <c r="S16" s="6">
         <f xml:space="preserve"> 16022223.4 / 1000</f>
         <v>16022.223400000001</v>
       </c>
@@ -1597,43 +1589,43 @@
       <c r="F17" s="2">
         <v>41288</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>25.9</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="7">
+      <c r="H17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="6">
         <v>6649.3</v>
       </c>
-      <c r="M17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="7">
+      <c r="M17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="6">
         <v>10838</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="6">
         <v>63344.5</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="6">
         <v>2696.5</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="6">
         <v>165.1</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R17" s="6">
         <v>1535</v>
       </c>
-      <c r="S17" s="7">
+      <c r="S17" s="6">
         <f xml:space="preserve"> 14877213.8 / 1000</f>
         <v>14877.213800000001</v>
       </c>
@@ -1664,43 +1656,43 @@
       <c r="F18" s="2">
         <v>37629.5</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>25.9</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="7">
+      <c r="H18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="6">
         <v>7320.8</v>
       </c>
-      <c r="M18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="7">
+      <c r="M18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="6">
         <v>10551</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="6">
         <v>60117.7</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="6">
         <v>1270</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q18" s="6">
         <v>138.69999999999999</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R18" s="6">
         <v>1684</v>
       </c>
-      <c r="S18" s="7">
+      <c r="S18" s="6">
         <f xml:space="preserve"> 13562423.7 / 1000</f>
         <v>13562.423699999999</v>
       </c>
@@ -1731,46 +1723,46 @@
       <c r="F19" s="2">
         <v>34278.9</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>25.9</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="7">
+      <c r="H19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="6">
         <v>7689.2</v>
       </c>
-      <c r="M19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N19" s="7">
+      <c r="M19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="6">
         <v>10455</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="6">
         <v>57475.199999999997</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P19" s="6">
         <v>2335.9</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="Q19" s="6">
         <v>181.1</v>
       </c>
-      <c r="R19" s="7">
+      <c r="R19" s="6">
         <v>2530</v>
       </c>
-      <c r="S19" s="7">
+      <c r="S19" s="6">
         <v>31739</v>
       </c>
-      <c r="T19" s="7">
+      <c r="T19" s="6">
         <v>722</v>
       </c>
       <c r="U19" s="2">
@@ -1796,46 +1788,46 @@
       <c r="F20" s="2">
         <v>32674.7</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>25.9</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="7">
+      <c r="H20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="6">
         <f xml:space="preserve"> 4558593 / 1000</f>
         <v>4558.5929999999998</v>
       </c>
-      <c r="M20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="7">
+      <c r="M20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="6">
         <f xml:space="preserve"> 41975492 / 1000</f>
         <v>41975.491999999998</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="6">
         <f xml:space="preserve"> 3280900 / 1000</f>
         <v>3280.9</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="6">
         <v>123.8</v>
       </c>
-      <c r="R20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S20" s="7">
+      <c r="R20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" s="6">
         <f xml:space="preserve"> 10145823.2 / 1000</f>
         <v>10145.823199999999</v>
       </c>
@@ -1866,43 +1858,43 @@
       <c r="F21" s="2">
         <v>45526</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>25.9</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="7">
+      <c r="H21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="6">
         <v>3022.6</v>
       </c>
-      <c r="M21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N21" s="7">
+      <c r="M21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="6">
         <v>5566</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="6">
         <v>22280.27</v>
       </c>
-      <c r="P21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S21" s="7">
+      <c r="P21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="6">
         <f>21358889.6/1000</f>
         <v>21358.889600000002</v>
       </c>
@@ -1933,43 +1925,43 @@
       <c r="F22" s="2">
         <v>41230.699999999997</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>25.9</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" s="7">
+      <c r="H22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="6">
         <v>12843.2</v>
       </c>
-      <c r="M22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N22" s="7">
+      <c r="M22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="6">
         <v>5245</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="6">
         <v>33385.4</v>
       </c>
-      <c r="P22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22" s="7">
+      <c r="P22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="6">
         <f>15613892/1000</f>
         <v>15613.892</v>
       </c>
@@ -2000,43 +1992,43 @@
       <c r="F23" s="2">
         <v>41319.300000000003</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>25.9</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="7">
+      <c r="H23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="6">
         <v>2983.3</v>
       </c>
-      <c r="M23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N23" s="7">
+      <c r="M23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="6">
         <v>5071</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="6">
         <v>26147.7</v>
       </c>
-      <c r="P23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S23" s="7">
+      <c r="P23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S23" s="6">
         <f xml:space="preserve"> 9892900 / 1000</f>
         <v>9892.9</v>
       </c>
@@ -2067,43 +2059,43 @@
       <c r="F24" s="2">
         <v>38178.1</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>25.9</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="7">
+      <c r="H24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="6">
         <v>4169.8</v>
       </c>
-      <c r="M24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N24" s="7">
+      <c r="M24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="6">
         <v>4979</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="6">
         <v>25080.5</v>
       </c>
-      <c r="P24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S24" s="7">
+      <c r="P24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S24" s="6">
         <f>9719218.2/1000</f>
         <v>9719.2181999999993</v>
       </c>
@@ -2125,7 +2117,7 @@
       <c r="C25" s="2">
         <v>194.703</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>41.1</v>
       </c>
       <c r="E25" s="2">
@@ -2134,46 +2126,46 @@
       <c r="F25" s="2">
         <v>77711</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>32.299999999999997</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="7">
+      <c r="H25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="6">
         <f>32741549/1000</f>
         <v>32741.548999999999</v>
       </c>
-      <c r="M25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N25" s="7">
+      <c r="M25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="6">
         <v>6928</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O25" s="6">
         <f xml:space="preserve"> 188.5 * 1000</f>
         <v>188500</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="6">
         <f>2.8*1000</f>
         <v>2800</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="Q25" s="6">
         <v>301.2</v>
       </c>
-      <c r="R25" s="7">
+      <c r="R25" s="6">
         <v>2056</v>
       </c>
-      <c r="S25" s="7">
+      <c r="S25" s="6">
         <v>34208.9</v>
       </c>
       <c r="T25" s="2">
@@ -2193,7 +2185,7 @@
       <c r="C26" s="2">
         <v>192.55699999999999</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>42.4</v>
       </c>
       <c r="E26" s="2">
@@ -2202,45 +2194,45 @@
       <c r="F26" s="2">
         <v>69206</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>32.299999999999997</v>
       </c>
-      <c r="H26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="7">
+      <c r="H26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="6">
         <f>22754436/1000</f>
         <v>22754.436000000002</v>
       </c>
-      <c r="M26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N26" s="7">
+      <c r="M26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="6">
         <v>6566</v>
       </c>
-      <c r="O26" s="7">
+      <c r="O26" s="6">
         <f xml:space="preserve"> 172 * 1000</f>
         <v>172000</v>
       </c>
-      <c r="P26" s="7">
+      <c r="P26" s="6">
         <v>3002.7</v>
       </c>
-      <c r="Q26" s="7">
+      <c r="Q26" s="6">
         <v>282.5</v>
       </c>
-      <c r="R26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S26" s="7">
+      <c r="R26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="6">
         <f xml:space="preserve"> 33764801.6 /1000</f>
         <v>33764.801599999999</v>
       </c>
@@ -2262,7 +2254,7 @@
       <c r="C27" s="2">
         <v>193.827</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>41.5</v>
       </c>
       <c r="E27" s="2">
@@ -2271,45 +2263,45 @@
       <c r="F27" s="2">
         <v>61131</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>32.299999999999997</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="7">
+      <c r="H27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="6">
         <f>19495388/1000</f>
         <v>19495.387999999999</v>
       </c>
-      <c r="M27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N27" s="7">
+      <c r="M27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="6">
         <v>6511</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O27" s="6">
         <f xml:space="preserve"> 152.7 * 1000</f>
         <v>152700</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="6">
         <v>5924.4</v>
       </c>
-      <c r="Q27" s="7">
+      <c r="Q27" s="6">
         <v>321.89999999999998</v>
       </c>
-      <c r="R27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S27" s="7">
+      <c r="R27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" s="6">
         <f xml:space="preserve"> 30160128.5 /1000</f>
         <v>30160.128499999999</v>
       </c>
@@ -2331,7 +2323,7 @@
       <c r="C28" s="2">
         <v>195.833</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>41</v>
       </c>
       <c r="E28" s="2">
@@ -2340,45 +2332,45 @@
       <c r="F28" s="2">
         <v>56640</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>29.3</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="7">
+      <c r="H28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="6">
         <v>37458.699999999997</v>
       </c>
-      <c r="M28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N28" s="7">
+      <c r="M28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" s="6">
         <v>6442</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="6">
         <f xml:space="preserve"> 110.9 * 1000</f>
         <v>110900</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="6">
         <f xml:space="preserve"> 1589809 / 1000</f>
         <v>1589.809</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q28" s="6">
         <v>192.6</v>
       </c>
-      <c r="R28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S28" s="7">
+      <c r="R28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" s="6">
         <f>27435002/1000</f>
         <v>27435.002</v>
       </c>
@@ -2400,7 +2392,7 @@
       <c r="C29" s="2">
         <v>198.22900000000001</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>42.8</v>
       </c>
       <c r="E29" s="2">
@@ -2409,46 +2401,46 @@
       <c r="F29" s="2">
         <v>55350</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>28.6</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="7">
+      <c r="H29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="6">
         <f>21049559/1000</f>
         <v>21049.559000000001</v>
       </c>
-      <c r="M29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N29" s="7">
+      <c r="M29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="6">
         <v>6476</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="6">
         <f>101*1000</f>
         <v>101000</v>
       </c>
-      <c r="P29" s="7">
+      <c r="P29" s="6">
         <f xml:space="preserve"> 1573240 / 1000</f>
         <v>1573.24</v>
       </c>
-      <c r="Q29" s="7">
+      <c r="Q29" s="6">
         <v>193.08</v>
       </c>
-      <c r="R29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S29" s="7">
+      <c r="R29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="6">
         <f>24726130.6/1000</f>
         <v>24726.1306</v>
       </c>
@@ -2470,7 +2462,7 @@
       <c r="C30" s="2">
         <v>199.61099999999999</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>42.3</v>
       </c>
       <c r="E30" s="2">
@@ -2479,46 +2471,46 @@
       <c r="F30" s="2">
         <v>51266</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <v>27.5</v>
       </c>
-      <c r="H30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="7">
+      <c r="H30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="6">
         <f>26707512/1000</f>
         <v>26707.511999999999</v>
       </c>
-      <c r="M30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N30" s="7">
+      <c r="M30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="6">
         <v>6584</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="6">
         <f>105.7*1000</f>
         <v>105700</v>
       </c>
-      <c r="P30" s="8">
+      <c r="P30" s="7">
         <f>4153307.4/1000</f>
         <v>4153.3073999999997</v>
       </c>
-      <c r="Q30" s="7">
+      <c r="Q30" s="6">
         <v>121.1</v>
       </c>
-      <c r="R30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S30" s="7">
+      <c r="R30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S30" s="6">
         <f>14607097.9/1000</f>
         <v>14607.097900000001</v>
       </c>
@@ -2540,7 +2532,7 @@
       <c r="C31" s="2">
         <v>201.232</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>36.700000000000003</v>
       </c>
       <c r="E31" s="2">
@@ -2549,45 +2541,45 @@
       <c r="F31" s="2">
         <v>45530</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>26.9</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31" s="7">
+      <c r="H31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="6">
         <f>7232770/1000</f>
         <v>7232.77</v>
       </c>
-      <c r="M31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N31" s="7">
+      <c r="M31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="6">
         <v>8968</v>
       </c>
-      <c r="O31" s="7">
+      <c r="O31" s="6">
         <f>65.7 *1000</f>
         <v>65700</v>
       </c>
-      <c r="P31" s="7">
+      <c r="P31" s="6">
         <v>562.70000000000005</v>
       </c>
-      <c r="Q31" s="7">
+      <c r="Q31" s="6">
         <v>102.3</v>
       </c>
-      <c r="R31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S31" s="7">
+      <c r="R31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S31" s="6">
         <f>14037631.3/1000</f>
         <v>14037.631300000001</v>
       </c>
@@ -2618,44 +2610,44 @@
       <c r="F32" s="2">
         <v>52971</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="8">
         <v>27.3</v>
       </c>
-      <c r="H32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" s="7">
+      <c r="H32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" s="6">
         <f>12749153/1000</f>
         <v>12749.153</v>
       </c>
-      <c r="M32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N32" s="7">
+      <c r="M32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="6">
         <v>3606</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="6">
         <v>49354.7</v>
       </c>
-      <c r="P32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q32" s="7">
+      <c r="P32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q32" s="6">
         <v>0</v>
       </c>
-      <c r="R32" s="7">
+      <c r="R32" s="6">
         <v>0</v>
       </c>
-      <c r="S32" s="7">
+      <c r="S32" s="6">
         <f>24179709.1/1000</f>
         <v>24179.7091</v>
       </c>
@@ -2668,31 +2660,138 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C33" s="2">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="D33" s="2">
+        <v>14.8</v>
+      </c>
+      <c r="E33" s="2">
+        <v>311</v>
+      </c>
+      <c r="F33" s="2">
+        <v>28993.5</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" s="6">
+        <v>945.42700000000002</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O33" s="6">
+        <v>9164.8922000000002</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S33" s="6">
+        <v>747.80160000000001</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U33" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C34" s="2">
+        <v>34.22</v>
+      </c>
+      <c r="D34" s="2">
+        <v>14.84</v>
+      </c>
+      <c r="E34" s="2">
+        <v>254</v>
+      </c>
+      <c r="F34" s="2">
+        <v>26864.3</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="2">
+        <v>782.58500000000004</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O34" s="2">
+        <v>9026.0113999999994</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S34" s="2">
+        <v>352.14210000000003</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U34" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2714,8 +2813,8 @@
       <c r="U35" s="2"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2737,8 +2836,8 @@
       <c r="U36" s="2"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2760,8 +2859,8 @@
       <c r="U38" s="2"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2783,8 +2882,8 @@
       <c r="U39" s="2"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2806,8 +2905,8 @@
       <c r="U40" s="2"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2829,8 +2928,8 @@
       <c r="U42" s="2"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2852,8 +2951,8 @@
       <c r="U43" s="2"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2875,8 +2974,8 @@
       <c r="U45" s="2"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2898,8 +2997,8 @@
       <c r="U46" s="2"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2921,8 +3020,8 @@
       <c r="U47" s="2"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2944,8 +3043,8 @@
       <c r="U49" s="2"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>

</xml_diff>

<commit_message>
Azov city 17-18 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -110,25 +110,20 @@
   <si>
     <t>Сланцы</t>
   </si>
+  <si>
+    <t>Азов</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -184,15 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -205,7 +197,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -490,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +690,7 @@
         <f xml:space="preserve"> 35242373 / 1000</f>
         <v>35242.373</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <f xml:space="preserve"> 3936 / 1000</f>
         <v>3.9359999999999999</v>
       </c>
@@ -766,7 +758,7 @@
       <c r="O4" s="2">
         <v>35244.355000000003</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="5">
         <f xml:space="preserve"> 5651769 / 1000</f>
         <v>5651.7690000000002</v>
       </c>
@@ -832,7 +824,7 @@
       <c r="O5" s="2">
         <v>28569.743999999999</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>1633.874</v>
       </c>
       <c r="Q5" s="2" t="s">
@@ -1455,43 +1447,43 @@
       <c r="F15" s="2">
         <v>47095.7</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>25.9</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="6">
+      <c r="H15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="5">
         <v>8534.4</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="6">
+      <c r="M15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="5">
         <v>11911</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="5">
         <v>98966.3</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="5">
         <v>10252.700000000001</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15" s="5">
         <v>88.7</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15" s="5">
         <v>1340</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="5">
         <f xml:space="preserve"> 22883164.3 / 1000</f>
         <v>22883.1643</v>
       </c>
@@ -1522,43 +1514,43 @@
       <c r="F16" s="2">
         <v>43057.3</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>25.9</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="6">
+      <c r="H16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="5">
         <v>19293.900000000001</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="6">
+      <c r="M16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="5">
         <v>11312</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="5">
         <v>81900</v>
       </c>
-      <c r="P16" s="6">
+      <c r="P16" s="5">
         <v>8500</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="Q16" s="5">
         <v>142.5</v>
       </c>
-      <c r="R16" s="6">
+      <c r="R16" s="5">
         <v>646</v>
       </c>
-      <c r="S16" s="6">
+      <c r="S16" s="5">
         <f xml:space="preserve"> 16022223.4 / 1000</f>
         <v>16022.223400000001</v>
       </c>
@@ -1589,43 +1581,43 @@
       <c r="F17" s="2">
         <v>41288</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>25.9</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="6">
+      <c r="H17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="5">
         <v>6649.3</v>
       </c>
-      <c r="M17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="6">
+      <c r="M17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="5">
         <v>10838</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="5">
         <v>63344.5</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P17" s="5">
         <v>2696.5</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q17" s="5">
         <v>165.1</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R17" s="5">
         <v>1535</v>
       </c>
-      <c r="S17" s="6">
+      <c r="S17" s="5">
         <f xml:space="preserve"> 14877213.8 / 1000</f>
         <v>14877.213800000001</v>
       </c>
@@ -1656,43 +1648,43 @@
       <c r="F18" s="2">
         <v>37629.5</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>25.9</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="6">
+      <c r="H18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="5">
         <v>7320.8</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="6">
+      <c r="M18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="5">
         <v>10551</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="5">
         <v>60117.7</v>
       </c>
-      <c r="P18" s="6">
+      <c r="P18" s="5">
         <v>1270</v>
       </c>
-      <c r="Q18" s="6">
+      <c r="Q18" s="5">
         <v>138.69999999999999</v>
       </c>
-      <c r="R18" s="6">
+      <c r="R18" s="5">
         <v>1684</v>
       </c>
-      <c r="S18" s="6">
+      <c r="S18" s="5">
         <f xml:space="preserve"> 13562423.7 / 1000</f>
         <v>13562.423699999999</v>
       </c>
@@ -1723,46 +1715,46 @@
       <c r="F19" s="2">
         <v>34278.9</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>25.9</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="6">
+      <c r="H19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="5">
         <v>7689.2</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N19" s="6">
+      <c r="M19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="5">
         <v>10455</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="5">
         <v>57475.199999999997</v>
       </c>
-      <c r="P19" s="6">
+      <c r="P19" s="5">
         <v>2335.9</v>
       </c>
-      <c r="Q19" s="6">
+      <c r="Q19" s="5">
         <v>181.1</v>
       </c>
-      <c r="R19" s="6">
+      <c r="R19" s="5">
         <v>2530</v>
       </c>
-      <c r="S19" s="6">
+      <c r="S19" s="5">
         <v>31739</v>
       </c>
-      <c r="T19" s="6">
+      <c r="T19" s="5">
         <v>722</v>
       </c>
       <c r="U19" s="2">
@@ -1788,46 +1780,46 @@
       <c r="F20" s="2">
         <v>32674.7</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>25.9</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="6">
+      <c r="H20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="5">
         <f xml:space="preserve"> 4558593 / 1000</f>
         <v>4558.5929999999998</v>
       </c>
-      <c r="M20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="6">
+      <c r="M20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="5">
         <f xml:space="preserve"> 41975492 / 1000</f>
         <v>41975.491999999998</v>
       </c>
-      <c r="P20" s="6">
+      <c r="P20" s="5">
         <f xml:space="preserve"> 3280900 / 1000</f>
         <v>3280.9</v>
       </c>
-      <c r="Q20" s="6">
+      <c r="Q20" s="5">
         <v>123.8</v>
       </c>
-      <c r="R20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S20" s="6">
+      <c r="R20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" s="5">
         <f xml:space="preserve"> 10145823.2 / 1000</f>
         <v>10145.823199999999</v>
       </c>
@@ -1858,43 +1850,43 @@
       <c r="F21" s="2">
         <v>45526</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>25.9</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="6">
+      <c r="H21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="5">
         <v>3022.6</v>
       </c>
-      <c r="M21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N21" s="6">
+      <c r="M21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="5">
         <v>5566</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="5">
         <v>22280.27</v>
       </c>
-      <c r="P21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S21" s="6">
+      <c r="P21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="5">
         <f>21358889.6/1000</f>
         <v>21358.889600000002</v>
       </c>
@@ -1925,43 +1917,43 @@
       <c r="F22" s="2">
         <v>41230.699999999997</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>25.9</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" s="6">
+      <c r="H22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="5">
         <v>12843.2</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N22" s="6">
+      <c r="M22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="5">
         <v>5245</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="5">
         <v>33385.4</v>
       </c>
-      <c r="P22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22" s="6">
+      <c r="P22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="5">
         <f>15613892/1000</f>
         <v>15613.892</v>
       </c>
@@ -1992,43 +1984,43 @@
       <c r="F23" s="2">
         <v>41319.300000000003</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <v>25.9</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="6">
+      <c r="H23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="5">
         <v>2983.3</v>
       </c>
-      <c r="M23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N23" s="6">
+      <c r="M23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="5">
         <v>5071</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="5">
         <v>26147.7</v>
       </c>
-      <c r="P23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S23" s="6">
+      <c r="P23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S23" s="5">
         <f xml:space="preserve"> 9892900 / 1000</f>
         <v>9892.9</v>
       </c>
@@ -2059,43 +2051,43 @@
       <c r="F24" s="2">
         <v>38178.1</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>25.9</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="6">
+      <c r="H24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="5">
         <v>4169.8</v>
       </c>
-      <c r="M24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N24" s="6">
+      <c r="M24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="5">
         <v>4979</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="5">
         <v>25080.5</v>
       </c>
-      <c r="P24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S24" s="6">
+      <c r="P24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S24" s="5">
         <f>9719218.2/1000</f>
         <v>9719.2181999999993</v>
       </c>
@@ -2117,7 +2109,7 @@
       <c r="C25" s="2">
         <v>194.703</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>41.1</v>
       </c>
       <c r="E25" s="2">
@@ -2126,46 +2118,46 @@
       <c r="F25" s="2">
         <v>77711</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>32.299999999999997</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="6">
+      <c r="H25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="5">
         <f>32741549/1000</f>
         <v>32741.548999999999</v>
       </c>
-      <c r="M25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N25" s="6">
+      <c r="M25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="5">
         <v>6928</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="5">
         <f xml:space="preserve"> 188.5 * 1000</f>
         <v>188500</v>
       </c>
-      <c r="P25" s="6">
+      <c r="P25" s="5">
         <f>2.8*1000</f>
         <v>2800</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="Q25" s="5">
         <v>301.2</v>
       </c>
-      <c r="R25" s="6">
+      <c r="R25" s="5">
         <v>2056</v>
       </c>
-      <c r="S25" s="6">
+      <c r="S25" s="5">
         <v>34208.9</v>
       </c>
       <c r="T25" s="2">
@@ -2185,7 +2177,7 @@
       <c r="C26" s="2">
         <v>192.55699999999999</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>42.4</v>
       </c>
       <c r="E26" s="2">
@@ -2194,45 +2186,45 @@
       <c r="F26" s="2">
         <v>69206</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="5">
         <v>32.299999999999997</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="6">
+      <c r="H26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="5">
         <f>22754436/1000</f>
         <v>22754.436000000002</v>
       </c>
-      <c r="M26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N26" s="6">
+      <c r="M26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="5">
         <v>6566</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="5">
         <f xml:space="preserve"> 172 * 1000</f>
         <v>172000</v>
       </c>
-      <c r="P26" s="6">
+      <c r="P26" s="5">
         <v>3002.7</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="Q26" s="5">
         <v>282.5</v>
       </c>
-      <c r="R26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S26" s="6">
+      <c r="R26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="5">
         <f xml:space="preserve"> 33764801.6 /1000</f>
         <v>33764.801599999999</v>
       </c>
@@ -2254,7 +2246,7 @@
       <c r="C27" s="2">
         <v>193.827</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>41.5</v>
       </c>
       <c r="E27" s="2">
@@ -2263,45 +2255,45 @@
       <c r="F27" s="2">
         <v>61131</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>32.299999999999997</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="6">
+      <c r="H27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="5">
         <f>19495388/1000</f>
         <v>19495.387999999999</v>
       </c>
-      <c r="M27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N27" s="6">
+      <c r="M27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="5">
         <v>6511</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="5">
         <f xml:space="preserve"> 152.7 * 1000</f>
         <v>152700</v>
       </c>
-      <c r="P27" s="6">
+      <c r="P27" s="5">
         <v>5924.4</v>
       </c>
-      <c r="Q27" s="6">
+      <c r="Q27" s="5">
         <v>321.89999999999998</v>
       </c>
-      <c r="R27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S27" s="6">
+      <c r="R27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" s="5">
         <f xml:space="preserve"> 30160128.5 /1000</f>
         <v>30160.128499999999</v>
       </c>
@@ -2323,7 +2315,7 @@
       <c r="C28" s="2">
         <v>195.833</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>41</v>
       </c>
       <c r="E28" s="2">
@@ -2332,45 +2324,45 @@
       <c r="F28" s="2">
         <v>56640</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="5">
         <v>29.3</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="6">
+      <c r="H28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="5">
         <v>37458.699999999997</v>
       </c>
-      <c r="M28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N28" s="6">
+      <c r="M28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" s="5">
         <v>6442</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="5">
         <f xml:space="preserve"> 110.9 * 1000</f>
         <v>110900</v>
       </c>
-      <c r="P28" s="6">
+      <c r="P28" s="5">
         <f xml:space="preserve"> 1589809 / 1000</f>
         <v>1589.809</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="Q28" s="5">
         <v>192.6</v>
       </c>
-      <c r="R28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S28" s="6">
+      <c r="R28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" s="5">
         <f>27435002/1000</f>
         <v>27435.002</v>
       </c>
@@ -2392,7 +2384,7 @@
       <c r="C29" s="2">
         <v>198.22900000000001</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>42.8</v>
       </c>
       <c r="E29" s="2">
@@ -2401,46 +2393,46 @@
       <c r="F29" s="2">
         <v>55350</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>28.6</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="6">
+      <c r="H29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="5">
         <f>21049559/1000</f>
         <v>21049.559000000001</v>
       </c>
-      <c r="M29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N29" s="6">
+      <c r="M29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="5">
         <v>6476</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O29" s="5">
         <f>101*1000</f>
         <v>101000</v>
       </c>
-      <c r="P29" s="6">
+      <c r="P29" s="5">
         <f xml:space="preserve"> 1573240 / 1000</f>
         <v>1573.24</v>
       </c>
-      <c r="Q29" s="6">
+      <c r="Q29" s="5">
         <v>193.08</v>
       </c>
-      <c r="R29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S29" s="6">
+      <c r="R29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="5">
         <f>24726130.6/1000</f>
         <v>24726.1306</v>
       </c>
@@ -2462,7 +2454,7 @@
       <c r="C30" s="2">
         <v>199.61099999999999</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>42.3</v>
       </c>
       <c r="E30" s="2">
@@ -2471,46 +2463,46 @@
       <c r="F30" s="2">
         <v>51266</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <v>27.5</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="6">
+      <c r="H30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="5">
         <f>26707512/1000</f>
         <v>26707.511999999999</v>
       </c>
-      <c r="M30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N30" s="6">
+      <c r="M30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="5">
         <v>6584</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O30" s="5">
         <f>105.7*1000</f>
         <v>105700</v>
       </c>
-      <c r="P30" s="7">
+      <c r="P30" s="6">
         <f>4153307.4/1000</f>
         <v>4153.3073999999997</v>
       </c>
-      <c r="Q30" s="6">
+      <c r="Q30" s="5">
         <v>121.1</v>
       </c>
-      <c r="R30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S30" s="6">
+      <c r="R30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S30" s="5">
         <f>14607097.9/1000</f>
         <v>14607.097900000001</v>
       </c>
@@ -2532,7 +2524,7 @@
       <c r="C31" s="2">
         <v>201.232</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>36.700000000000003</v>
       </c>
       <c r="E31" s="2">
@@ -2541,45 +2533,45 @@
       <c r="F31" s="2">
         <v>45530</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <v>26.9</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31" s="6">
+      <c r="H31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="5">
         <f>7232770/1000</f>
         <v>7232.77</v>
       </c>
-      <c r="M31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N31" s="6">
+      <c r="M31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="5">
         <v>8968</v>
       </c>
-      <c r="O31" s="6">
+      <c r="O31" s="5">
         <f>65.7 *1000</f>
         <v>65700</v>
       </c>
-      <c r="P31" s="6">
+      <c r="P31" s="5">
         <v>562.70000000000005</v>
       </c>
-      <c r="Q31" s="6">
+      <c r="Q31" s="5">
         <v>102.3</v>
       </c>
-      <c r="R31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S31" s="6">
+      <c r="R31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S31" s="5">
         <f>14037631.3/1000</f>
         <v>14037.631300000001</v>
       </c>
@@ -2610,44 +2602,44 @@
       <c r="F32" s="2">
         <v>52971</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="7">
         <v>27.3</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" s="6">
+      <c r="H32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" s="5">
         <f>12749153/1000</f>
         <v>12749.153</v>
       </c>
-      <c r="M32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N32" s="6">
+      <c r="M32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="5">
         <v>3606</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="5">
         <v>49354.7</v>
       </c>
-      <c r="P32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q32" s="6">
+      <c r="P32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q32" s="5">
         <v>0</v>
       </c>
-      <c r="R32" s="6">
+      <c r="R32" s="5">
         <v>0</v>
       </c>
-      <c r="S32" s="6">
+      <c r="S32" s="5">
         <f>24179709.1/1000</f>
         <v>24179.7091</v>
       </c>
@@ -2678,43 +2670,43 @@
       <c r="F33" s="2">
         <v>28993.5</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L33" s="6">
+      <c r="G33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" s="5">
         <v>945.42700000000002</v>
       </c>
-      <c r="M33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O33" s="6">
+      <c r="M33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O33" s="5">
         <v>9164.8922000000002</v>
       </c>
-      <c r="P33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S33" s="6">
+      <c r="P33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S33" s="5">
         <v>747.80160000000001</v>
       </c>
       <c r="T33" s="2" t="s">
@@ -2743,40 +2735,40 @@
       <c r="F34" s="2">
         <v>26864.3</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K34" s="6" t="s">
+      <c r="G34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="5" t="s">
         <v>22</v>
       </c>
       <c r="L34" s="2">
         <v>782.58500000000004</v>
       </c>
-      <c r="M34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N34" s="6" t="s">
+      <c r="M34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="5" t="s">
         <v>22</v>
       </c>
       <c r="O34" s="2">
         <v>9026.0113999999994</v>
       </c>
-      <c r="P34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R34" s="6" t="s">
+      <c r="P34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R34" s="5" t="s">
         <v>22</v>
       </c>
       <c r="S34" s="2">
@@ -2790,100 +2782,143 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
+      <c r="A35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C35" s="2">
+        <v>80.721000000000004</v>
+      </c>
+      <c r="D35" s="2">
+        <v>17.966999999999999</v>
+      </c>
+      <c r="E35" s="2">
+        <v>296</v>
+      </c>
+      <c r="F35" s="2">
+        <v>29249.1</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" s="2">
+        <v>3672</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O35" s="2">
+        <f xml:space="preserve"> 28823135 / 1000</f>
+        <v>28823.134999999998</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>60</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S35" s="2">
+        <v>12216.4</v>
+      </c>
+      <c r="T35" s="2">
+        <v>413.2</v>
+      </c>
+      <c r="U35" s="2">
+        <v>-51</v>
+      </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
+      <c r="A36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C36" s="2">
+        <v>81.355000000000004</v>
+      </c>
+      <c r="D36" s="2">
+        <v>17.454999999999998</v>
+      </c>
+      <c r="E36" s="2">
+        <v>290</v>
+      </c>
+      <c r="F36" s="2">
+        <v>27044.2</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="2">
+        <v>3050.8</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O36" s="2">
+        <f xml:space="preserve"> 29006627.2/1000</f>
+        <v>29006.627199999999</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>66.543000000000006</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S36" s="2">
+        <v>11765.9</v>
+      </c>
+      <c r="T36" s="2">
+        <v>399.8</v>
+      </c>
+      <c r="U36" s="2">
+        <v>-206</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2905,8 +2940,8 @@
       <c r="U40" s="2"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2928,8 +2963,8 @@
       <c r="U42" s="2"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2951,8 +2986,8 @@
       <c r="U43" s="2"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2974,8 +3009,8 @@
       <c r="U45" s="2"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2997,8 +3032,8 @@
       <c r="U46" s="2"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -3020,8 +3055,8 @@
       <c r="U47" s="2"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -3043,8 +3078,8 @@
       <c r="U49" s="2"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>

</xml_diff>

<commit_message>
Get max. values of features
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -483,7 +483,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2786,65 +2786,41 @@
         <v>30</v>
       </c>
       <c r="B35" s="1">
-        <v>2018</v>
-      </c>
-      <c r="C35" s="2">
-        <v>80.721000000000004</v>
+        <v>2022</v>
       </c>
       <c r="D35" s="2">
-        <v>17.966999999999999</v>
+        <v>16.709</v>
       </c>
       <c r="E35" s="2">
-        <v>296</v>
+        <v>249</v>
       </c>
       <c r="F35" s="2">
-        <v>29249.1</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>22</v>
+        <v>42183.9</v>
       </c>
       <c r="L35" s="2">
-        <v>3672</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>22</v>
+        <v>7457.5</v>
       </c>
       <c r="O35" s="2">
-        <f xml:space="preserve"> 28823135 / 1000</f>
-        <v>28823.134999999998</v>
+        <f xml:space="preserve"> 31930746 / 1000</f>
+        <v>31930.745999999999</v>
       </c>
       <c r="P35" s="5" t="s">
         <v>22</v>
       </c>
       <c r="Q35" s="5">
-        <v>60</v>
+        <v>24.47</v>
       </c>
       <c r="R35" s="5" t="s">
         <v>22</v>
       </c>
       <c r="S35" s="2">
-        <v>12216.4</v>
+        <v>18312</v>
       </c>
       <c r="T35" s="2">
-        <v>413.2</v>
+        <v>486.4</v>
       </c>
       <c r="U35" s="2">
-        <v>-51</v>
+        <v>-232</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -2852,69 +2828,132 @@
         <v>30</v>
       </c>
       <c r="B36" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C36" s="2">
+        <v>80.721000000000004</v>
+      </c>
+      <c r="D36" s="2">
+        <v>17.966999999999999</v>
+      </c>
+      <c r="E36" s="2">
+        <v>296</v>
+      </c>
+      <c r="F36" s="2">
+        <v>29249.1</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="2">
+        <v>3672</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O36" s="2">
+        <f xml:space="preserve"> 28823135 / 1000</f>
+        <v>28823.134999999998</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>60</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S36" s="2">
+        <v>12216.4</v>
+      </c>
+      <c r="T36" s="2">
+        <v>413.2</v>
+      </c>
+      <c r="U36" s="2">
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="1">
         <v>2017</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C37" s="2">
         <v>81.355000000000004</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D37" s="2">
         <v>17.454999999999998</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E37" s="2">
         <v>290</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F37" s="2">
         <v>27044.2</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L36" s="2">
+      <c r="G37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="2">
         <v>3050.8</v>
       </c>
-      <c r="M36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O36" s="2">
+      <c r="M37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O37" s="2">
         <f xml:space="preserve"> 29006627.2/1000</f>
         <v>29006.627199999999</v>
       </c>
-      <c r="P36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q36" s="5">
+      <c r="P37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q37" s="5">
         <v>66.543000000000006</v>
       </c>
-      <c r="R36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="S36" s="2">
+      <c r="R37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S37" s="2">
         <v>11765.9</v>
       </c>
-      <c r="T36" s="2">
+      <c r="T37" s="2">
         <v>399.8</v>
       </c>
-      <c r="U36" s="2">
+      <c r="U37" s="2">
         <v>-206</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>

</xml_diff>

<commit_message>
RO dist. small cities (2018)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>Азов</t>
+  </si>
+  <si>
+    <t>Гуково</t>
+  </si>
+  <si>
+    <t>Донецк</t>
+  </si>
+  <si>
+    <t>Каменск-Шахтинский</t>
+  </si>
+  <si>
+    <t>Зверево</t>
   </si>
 </sst>
 </file>
@@ -482,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2797,6 +2809,21 @@
       <c r="F35" s="2">
         <v>42183.9</v>
       </c>
+      <c r="G35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="L35" s="2">
         <v>7457.5</v>
       </c>
@@ -2955,28 +2982,277 @@
         <v>-206</v>
       </c>
     </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C38" s="2">
+        <v>64.869</v>
+      </c>
+      <c r="D38" s="2">
+        <v>8.4819999999999993</v>
+      </c>
+      <c r="E38" s="2">
+        <v>958</v>
+      </c>
+      <c r="F38" s="2">
+        <v>22958.3</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O38" s="2">
+        <f xml:space="preserve"> 774396 / 1000</f>
+        <v>774.39599999999996</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q38" s="2">
+        <f xml:space="preserve"> 8137 / 1000</f>
+        <v>8.1370000000000005</v>
+      </c>
+      <c r="R38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S38" s="2">
+        <f xml:space="preserve"> 6362296.4 / 1000</f>
+        <v>6362.2964000000002</v>
+      </c>
+      <c r="T38" s="2">
+        <f xml:space="preserve"> 221935.5 / 1000</f>
+        <v>221.93549999999999</v>
+      </c>
+      <c r="U38" s="2">
+        <v>-403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C39" s="2">
+        <v>47770</v>
+      </c>
+      <c r="D39" s="2">
+        <v>6.41</v>
+      </c>
+      <c r="E39" s="2">
+        <v>523</v>
+      </c>
+      <c r="F39" s="2">
+        <v>21351</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O39" s="2">
+        <f>2584304/1000</f>
+        <v>2584.3040000000001</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>7.3150000000000004</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S39" s="2">
+        <f>4911240.3/1000</f>
+        <v>4911.2402999999995</v>
+      </c>
+      <c r="T39" s="2">
+        <f>138739.6/1000</f>
+        <v>138.7396</v>
+      </c>
+      <c r="U39" s="2">
+        <v>-197</v>
+      </c>
+    </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
+      <c r="A40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C40" s="2">
+        <v>88.997</v>
+      </c>
+      <c r="D40" s="2">
+        <v>27.875</v>
+      </c>
+      <c r="E40" s="2">
+        <v>753</v>
+      </c>
+      <c r="F40" s="2">
+        <v>28590.400000000001</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O40" s="2">
+        <f>20336870 / 1000</f>
+        <v>20336.87</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>16.305</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S40" s="2">
+        <f>17686635.8/1000</f>
+        <v>17686.6358</v>
+      </c>
+      <c r="T40" s="2">
+        <f>742584.8/1000</f>
+        <v>742.58480000000009</v>
+      </c>
+      <c r="U40" s="2">
+        <v>-71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C41" s="2">
+        <v>19.045000000000002</v>
+      </c>
+      <c r="D41" s="2">
+        <v>5.3419999999999996</v>
+      </c>
+      <c r="E41" s="2">
+        <v>382</v>
+      </c>
+      <c r="F41" s="2">
+        <v>27277.200000000001</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O41" s="2">
+        <v>209.60300000000001</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>2.024</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S41" s="2">
+        <f>1957826.5/1000</f>
+        <v>1957.8264999999999</v>
+      </c>
+      <c r="T41" s="2">
+        <f>53897.4/1000</f>
+        <v>53.897400000000005</v>
+      </c>
+      <c r="U41" s="2">
+        <v>-83</v>
+      </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>

</xml_diff>

<commit_message>
Rostov dist. data & dell. incorr. input
</commit_message>
<xml_diff>
--- a/migforecasting/less100/citiesless100 (raw data).xlsx
+++ b/migforecasting/less100/citiesless100 (raw data).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -495,7 +495,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,6 +2827,12 @@
       <c r="L35" s="2">
         <v>7457.5</v>
       </c>
+      <c r="M35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="O35" s="2">
         <f xml:space="preserve"> 31930746 / 1000</f>
         <v>31930.745999999999</v>

</xml_diff>